<commit_message>
modified:   ISPD2025_benchmarks/results/test.xlsx 	deleted:    ISPD2025_benchmarks/results/~$test.xlsx 	modified:   ISPD2025_benchmarks/run_ariane.tcl 	new file:   dev 	modified:   route/cugr2/GlobalRouter.cpp
</commit_message>
<xml_diff>
--- a/ISPD2025_benchmarks/results/test.xlsx
+++ b/ISPD2025_benchmarks/results/test.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\iris\work\route_sta\ISPD2025_benchmarks\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA716D9D-C83C-4D73-A7B2-DF0DB349B3AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BD0E46-4CDE-44E0-9D4F-FB80140A6A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="2010" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="ariane_fix" sheetId="2" r:id="rId2"/>
     <sheet name="bsg_chip" sheetId="3" r:id="rId3"/>
+    <sheet name="ariane_only_stg1" sheetId="4" r:id="rId4"/>
+    <sheet name="bsg_only_stg1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
   <si>
     <t>baseline</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,6 +88,10 @@
   </si>
   <si>
     <t>bsg_chip</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>of_after_stg1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -599,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A65974EE-4965-4794-8F23-8AACB855A855}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -773,139 +779,300 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E8504A-4AF7-465D-AE4D-22D3C6FC31EE}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1">
+        <v>110273</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1">
+        <v>935442</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>73636</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1">
+        <v>14985904.415411999</v>
+      </c>
+      <c r="C4" s="1">
+        <v>16399020.770132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1">
+        <v>15378268</v>
+      </c>
+      <c r="C5" s="1">
+        <v>16233372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>33277455.470692001</v>
+      </c>
+      <c r="C6" s="1">
+        <v>33448088.539326001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-0.39</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1">
+        <v>-6322.25</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-6742.87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2821</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48EF713-05C0-439D-8449-3B9024CD5357}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>15</v>
+      </c>
+      <c r="B2" s="1">
+        <v>26052</v>
+      </c>
+      <c r="C2" s="1">
+        <v>21487</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3767357.2043110002</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3767357.2043110002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3301836</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3297764</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10316379.26533</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10258074.674814999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-0.49</v>
+      </c>
+      <c r="C6" s="1">
+        <v>-0.49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1">
+        <v>-1210.6199999999999</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-1201.3699999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EF07B4-51F0-4183-8BE1-E83186FB1304}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="1">
         <v>110273</v>
       </c>
-      <c r="C2" s="1">
-        <v>21487</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1">
-        <v>935442</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1">
-        <v>73636</v>
+        <v>21497469.125300001</v>
       </c>
       <c r="C3" s="1">
-        <v>16252</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+        <v>21497469.125300001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>14985904.415411999</v>
+        <v>20866152</v>
       </c>
       <c r="C4" s="1">
-        <v>2586789.232084</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+        <v>20851260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
-        <v>15378268</v>
+        <v>34961494.361810997</v>
       </c>
       <c r="C5" s="1">
-        <v>2312696</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+        <v>34667571.438350998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>33277455.470692001</v>
+        <v>-0.42</v>
       </c>
       <c r="C6" s="1">
-        <v>9985988.1954069994</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+        <v>-0.42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
-        <v>-0.39</v>
+        <v>-8842.82</v>
       </c>
       <c r="C7" s="1">
-        <v>-0.4</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1">
-        <v>-6322.25</v>
-      </c>
-      <c r="C8" s="1">
-        <v>-6742.87</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2821</v>
-      </c>
-      <c r="C9" s="1">
-        <v>2407</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+        <v>-8767.32</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
update scripts new testcase/result merged branch "main"
</commit_message>
<xml_diff>
--- a/ISPD2025_benchmarks/results/test.xlsx
+++ b/ISPD2025_benchmarks/results/test.xlsx
@@ -8,28 +8,44 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\iris\work\route_sta\ISPD2025_benchmarks\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BD0E46-4CDE-44E0-9D4F-FB80140A6A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5199C6-424F-4A91-870B-4488892D6BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="ariane_fix" sheetId="2" r:id="rId2"/>
-    <sheet name="bsg_chip" sheetId="3" r:id="rId3"/>
-    <sheet name="ariane_only_stg1" sheetId="4" r:id="rId4"/>
-    <sheet name="bsg_only_stg1" sheetId="5" r:id="rId5"/>
+    <sheet name="ariane_fix" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="bsg_chip" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="ariane_only_stg1" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="bsg_only_stg1" sheetId="5" state="hidden" r:id="rId5"/>
+    <sheet name="ariane1" sheetId="8" state="hidden" r:id="rId6"/>
+    <sheet name="bsg1" sheetId="9" state="hidden" r:id="rId7"/>
+    <sheet name="ariane" sheetId="6" r:id="rId8"/>
+    <sheet name="bsg" sheetId="7" r:id="rId9"/>
+    <sheet name="nvdla" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="23">
   <si>
     <t>baseline</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -92,6 +108,34 @@
   </si>
   <si>
     <t>of_after_stg1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>of_after_stg2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tns%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wl%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>via%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>of%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wns%</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -99,7 +143,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,13 +164,31 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF79B8FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF986801"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -141,12 +203,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -430,7 +505,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -593,6 +668,265 @@
       </c>
       <c r="E9" s="1">
         <v>304</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703CA297-44F3-409E-9C97-EB1A56145966}">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6">
+        <v>39420</v>
+      </c>
+      <c r="C2" s="6">
+        <v>32819</v>
+      </c>
+      <c r="D2" s="3">
+        <v>39420</v>
+      </c>
+      <c r="E2" s="3">
+        <v>32819</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="3">
+        <v>27027</v>
+      </c>
+      <c r="E3" s="3">
+        <v>21533</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>10584203.181048</v>
+      </c>
+      <c r="C4" s="6">
+        <v>10584203.181048</v>
+      </c>
+      <c r="D4" s="3">
+        <v>10634829.780246001</v>
+      </c>
+      <c r="E4" s="3">
+        <v>10635227.675141999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6">
+        <v>4532436</v>
+      </c>
+      <c r="C5" s="6">
+        <v>4547984</v>
+      </c>
+      <c r="D5" s="3">
+        <v>4458748</v>
+      </c>
+      <c r="E5" s="3">
+        <v>4458128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>13771940.319569999</v>
+      </c>
+      <c r="C6" s="6">
+        <v>16026877.199145</v>
+      </c>
+      <c r="D6" s="3">
+        <v>11390349.502753001</v>
+      </c>
+      <c r="E6" s="3">
+        <v>11353387.711169999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <v>-141.37</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-141.34</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-141.36000000000001</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-141.36000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-852071.88</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-851804.31</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-852076.5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-852234.56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B12" si="0">B4/B4</f>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:E13" si="1">C4/B4</f>
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>1.0047832225375881</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1.0000374143173159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>1.0034303848967752</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>0.98037899869480627</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>0.99986094751262011</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>1.1637341454617491</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0.71070298731437531</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.996754990566877</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0.99978779090330339</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1.0001415027593039</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <f>B8/B8</f>
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f>C8/B8</f>
+        <v>0.99968597719713514</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1.0003195452251232</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>1.0001854997761352</v>
+      </c>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -899,7 +1233,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -992,8 +1326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35EF07B4-51F0-4183-8BE1-E83186FB1304}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1078,4 +1412,713 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B83DC53-88FE-428D-89B7-B12A28FB5630}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4">
+        <v>29860</v>
+      </c>
+      <c r="C2" s="4">
+        <v>24827</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>4919854.3363619996</v>
+      </c>
+      <c r="C4" s="4">
+        <v>4919854.3363619996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2946400</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2944084</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5436688.525041</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5353142.8809160003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>-0.47</v>
+      </c>
+      <c r="C7" s="4">
+        <v>-0.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>-1205.29</v>
+      </c>
+      <c r="C8" s="4">
+        <v>-1195.78</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83719EB-C256-40DF-8DEC-CB029E887D38}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="4">
+        <v>128156</v>
+      </c>
+      <c r="C2" s="4">
+        <v>98211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>27824640.866694</v>
+      </c>
+      <c r="C4" s="4">
+        <v>27824640.866694</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4">
+        <v>17525120</v>
+      </c>
+      <c r="C5" s="4">
+        <v>17516632</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>18316891.755509999</v>
+      </c>
+      <c r="C6" s="4">
+        <v>17963854.520435002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>-0.42</v>
+      </c>
+      <c r="C7" s="4">
+        <v>-0.42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>-8772.24</v>
+      </c>
+      <c r="C8" s="4">
+        <v>-8719.2800000000007</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8441568F-9AB9-4D02-A142-E2BA36155338}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6">
+        <v>29860</v>
+      </c>
+      <c r="C2" s="6">
+        <v>24827</v>
+      </c>
+      <c r="D2" s="3">
+        <v>29860</v>
+      </c>
+      <c r="E2" s="3">
+        <v>24827</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="3">
+        <v>24838</v>
+      </c>
+      <c r="E3" s="3">
+        <v>19969</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>4919854.3363619996</v>
+      </c>
+      <c r="C4" s="6">
+        <v>4919854.3363619996</v>
+      </c>
+      <c r="D4" s="3">
+        <v>4921661.4423479997</v>
+      </c>
+      <c r="E4" s="3">
+        <v>4921407.2317199996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6">
+        <v>2946400</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2944084</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2946528</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2947716</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>5436688.525041</v>
+      </c>
+      <c r="C6" s="6">
+        <v>5353142.8809160003</v>
+      </c>
+      <c r="D6" s="3">
+        <v>5369976.3360310001</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5315436.2483740002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <v>-0.47</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-0.47</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-0.47</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-0.47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-1205.29</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-1195.78</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-1203.3800000000001</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-1200.8599999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B12" si="0">B4/B4</f>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:E12" si="1">C4/B4</f>
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>1.0003673088393377</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0.99994834861540605</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0.99921395601411889</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>1.0008301393574368</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>1.0004031863942919</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.98463299051615805</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>1.0031445929035467</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.98984351433896434</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <f>B8/B8</f>
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f>C8/B8</f>
+        <v>0.99210978270789607</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:E13" si="2">D8/C8</f>
+        <v>1.0063556841559484</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>0.99790589838621202</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6861253-5D39-4D1D-81C8-82616229106C}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6">
+        <v>128156</v>
+      </c>
+      <c r="C2" s="6">
+        <v>98211</v>
+      </c>
+      <c r="D2" s="3">
+        <v>128156</v>
+      </c>
+      <c r="E2" s="3">
+        <v>98211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="3">
+        <v>96849</v>
+      </c>
+      <c r="E3" s="3">
+        <v>69688</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>27824640.866694</v>
+      </c>
+      <c r="C4" s="6">
+        <v>27824640.866694</v>
+      </c>
+      <c r="D4" s="3">
+        <v>27840976.662702002</v>
+      </c>
+      <c r="E4" s="3">
+        <v>27839639.293745998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6">
+        <v>17525120</v>
+      </c>
+      <c r="C5" s="6">
+        <v>17516632</v>
+      </c>
+      <c r="D5" s="3">
+        <v>17523896</v>
+      </c>
+      <c r="E5" s="3">
+        <v>17526332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>18316891.755509999</v>
+      </c>
+      <c r="C6" s="6">
+        <v>17963854.520435002</v>
+      </c>
+      <c r="D6" s="3">
+        <v>17945637.007975001</v>
+      </c>
+      <c r="E6" s="3">
+        <v>17749724.471258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <v>-0.42</v>
+      </c>
+      <c r="C7" s="6">
+        <v>-0.42</v>
+      </c>
+      <c r="D7" s="3">
+        <v>-0.42</v>
+      </c>
+      <c r="E7" s="3">
+        <v>-0.42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>-8772.24</v>
+      </c>
+      <c r="C8" s="6">
+        <v>-8719.2800000000007</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-8802.08</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-8809.36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <f t="shared" ref="B9:B12" si="0">B4/B4</f>
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:E13" si="1">C4/B4</f>
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>1.0005870981798566</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>0.99995196400714648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0.99951566665449365</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>1.0004146915913972</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>1.0001390101835801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.98072613848532475</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>0.99898587953719631</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>0.98908299902478036</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <f>B8/B8</f>
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <f>C8/B8</f>
+        <v>0.99396277347633</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>1.0094961969336917</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>1.0008270772362897</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new file:   ISPD2025_benchmarks/results/dev.txt 	modified:   ISPD2025_benchmarks/results/test.xlsx 	modified:   ISPD2025_benchmarks/run_ariane.tcl 	modified:   route/context/Context.cpp
</commit_message>
<xml_diff>
--- a/ISPD2025_benchmarks/results/test.xlsx
+++ b/ISPD2025_benchmarks/results/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\iris\work\route_sta\ISPD2025_benchmarks\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5199C6-424F-4A91-870B-4488892D6BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B48CB5D-C58F-4583-A669-77482A95E152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -226,7 +226,50 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -680,8 +723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{703CA297-44F3-409E-9C97-EB1A56145966}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1619,8 +1662,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8441568F-9AB9-4D02-A142-E2BA36155338}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1865,6 +1908,14 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A13:E13">
+    <cfRule type="top10" dxfId="4" priority="4" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="3" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A12:E12">
+    <cfRule type="top10" dxfId="0" priority="1" bottom="1" rank="1"/>
+    <cfRule type="top10" dxfId="1" priority="2" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1873,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6861253-5D39-4D1D-81C8-82616229106C}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>